<commit_message>
Finished an excel file with some test data
</commit_message>
<xml_diff>
--- a/JuddsProject/Validation/AdvanceRatio/UncertaintyValues.xlsx
+++ b/JuddsProject/Validation/AdvanceRatio/UncertaintyValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Desktop\FlowLab\JuddsProject\Validation\AdvanceRatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852726FD-A1CB-435E-885B-73F1BF78CBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9258A-E828-4BD1-9C83-E913E6BDE94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Variable</t>
   </si>
@@ -142,10 +142,28 @@
     <t>dv0/dtnet</t>
   </si>
   <si>
-    <t>dv0/du</t>
-  </si>
-  <si>
     <t>dv0/dvu</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>dv0/dqu</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>d_p</t>
+  </si>
+  <si>
+    <t>dJ/dv0</t>
+  </si>
+  <si>
+    <t>dJ/dn</t>
+  </si>
+  <si>
+    <t>dJ/dDp</t>
   </si>
 </sst>
 </file>
@@ -181,8 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,15 +637,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B69A33-2B1B-4385-8A7C-4B226C76146C}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -640,45 +662,82 @@
         <v>33</v>
       </c>
       <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <f>B12/2*B14^2</f>
+        <v>409.41750457414793</v>
+      </c>
       <c r="C2">
         <v>0.01</v>
       </c>
       <c r="F2">
         <f>(2*SQRT(2)*B6*B7*B8*B4)/(SQRT(B6*B7*B8*B4/((B3^2)*(B6-1)+2))*((B3^2)*(B6-1)+2))</f>
-        <v>12667.431164999474</v>
+        <v>2229.7255054557722</v>
       </c>
       <c r="G2">
         <f>SQRT(2)*B6*B7*B8*B3/(2*SQRT(B6*B7*B8*B4/((B3^2)*(B6-1)+2))*((B3^2)*(B6-1)+2))</f>
-        <v>3.4256669276325042</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.60298704782729518</v>
+      </c>
+      <c r="H2">
+        <f>(4*SQRT(B5/(B2*B11)+1)*(B9*B10*B14/(2*B11*SQRT(B5/(B2*B11)+1))) + 2*((B11^2)*B14/(B11*SQRT(B5/(B2*B11)+1))-B10*B14)-2*(B9*B10*B2*SQRT(B5/(B2*B11)+1) + 4*(B10^2)*B2*B14*SQRT(B5/(B2*B11)+1) - B10*B5*B14)/(B2*B11*SQRT(B5/(B2*B11)+1)))/(16*(B10^2)*B2*(B5/(B2*B11)+1))</f>
+        <v>-0.2821883892121072</v>
+      </c>
+      <c r="I2">
+        <f>(2*B2+(B5/B11))*(B14*B5/(8*B10*(B2^2 + B5*B2/B11)^(3/2)))</f>
+        <v>2.5391113700257511E-3</v>
+      </c>
+      <c r="J2">
+        <f>1+B9/(4*B10) - B5/(4*B10*B2*SQRT(1+B5/(B2*B11)))</f>
+        <v>1.0277736351672417</v>
+      </c>
+      <c r="K2">
+        <f>1/(B16*B15)</f>
+        <v>4.375368317137634E-3</v>
+      </c>
+      <c r="L2">
+        <f>-B13/((B16^2)*B15)</f>
+        <v>-3.2821035403725808E-2</v>
+      </c>
+      <c r="M2">
+        <f>-B13/(B16*(B15^2))</f>
+        <v>-1.2062347447624944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <f>0.6</f>
         <v>0.6</v>
       </c>
       <c r="C3">
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
+        <f>554.67</f>
         <v>554.66999999999996</v>
       </c>
       <c r="C4">
@@ -686,15 +745,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5">
+        <f>0.2383*B12*(B16^2)*(B11^4)</f>
+        <v>141.71827819739059</v>
+      </c>
       <c r="C5">
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -705,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -716,18 +779,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>1722</v>
+        <v>53.353000000000002</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -738,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -749,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -760,34 +823,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12">
-        <f>0.00183</f>
         <v>1.83E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>B14*(1+B9/(4*B10) - B5/(4*B10*B2*SQRT(1+B5/(B2*B11))))</f>
+        <v>687.49592645021835</v>
+      </c>
+      <c r="C13">
+        <f>SQRT((J2*C14)^2 + (I2*C2)^2 + (H2*C5)^2)</f>
+        <v>4.8531595402998358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14">
-        <f>B3*(B6*B7*B8*B4/(1+((B6-1)/2))*B3^2)^(0.5)</f>
-        <v>2155.101989185217</v>
+        <f>B3*SQRT((B6*B7*B8*B4)/(1+(((B6-1)/2)*(B3^2))))</f>
+        <v>668.91765163673165</v>
       </c>
       <c r="C14">
         <f>SQRT((F2*C3)^2 + (G2*C4)^2)</f>
-        <v>26.821271525233005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4.721089258713107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <f>29.925/12</f>
+        <v>2.4937499999999999</v>
+      </c>
+      <c r="C15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <f>5499/60</f>
+        <v>91.65</v>
+      </c>
+      <c r="C16" s="1">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <f>B13/(B16*B15)</f>
+        <v>3.0080478947514706</v>
+      </c>
+      <c r="C17">
+        <f>SQRT((K2*C13)^2 + (L2*C16)^2 + (M2*C15)^2)</f>
+        <v>2.1275626796528828E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Started my Hess-Smith panel method
</commit_message>
<xml_diff>
--- a/JuddsProject/Validation/AdvanceRatio/UncertaintyValues.xlsx
+++ b/JuddsProject/Validation/AdvanceRatio/UncertaintyValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Desktop\FlowLab\JuddsProject\Validation\AdvanceRatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9258A-E828-4BD1-9C83-E913E6BDE94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E4A18-DFAD-4CDB-84BE-8B3DEE22C834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3876" yWindow="1848" windowWidth="8916" windowHeight="7932" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B69A33-2B1B-4385-8A7C-4B226C76146C}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +879,7 @@
         <f>5499/60</f>
         <v>91.65</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>

</xml_diff>